<commit_message>
fix: pm, test 分值调整
</commit_message>
<xml_diff>
--- a/excel/绩效考核模板-测试.xlsx
+++ b/excel/绩效考核模板-测试.xlsx
@@ -126,14 +126,70 @@
         <color indexed="8"/>
         <rFont val="微软雅黑"/>
       </rPr>
-      <t>t &lt;= -8 (基数: 1.8) --8 &lt; t &lt;= -6 (基数: 1.5) --6 &lt; t &lt;= -3 (基数: 1.2) --3 &lt; t &lt;= 0 (基数: 1.0) -0 &lt; t &lt;= 2 (基数: 0.8) -2 &lt; t &lt;= 4 (基数: 0.6) -4 &lt; t &lt;= 6 (基数: 0.5) -t &gt; 6 (基数: 0)</t>
+      <t xml:space="preserve">t &lt;= -8 (基数: 1.8)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t xml:space="preserve">-8 &lt; t &lt;= -6 (基数: 1.5)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t xml:space="preserve">-6 &lt; t &lt;= -3 (基数: 1.2)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t xml:space="preserve">-3 &lt; t &lt;= 0 (基数: 1.0)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t xml:space="preserve">0 &lt; t &lt;= 2 (基数: 0.8)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t xml:space="preserve">2 &lt; t &lt;= 4 (基数: 0.6)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t xml:space="preserve">4 &lt; t &lt;= 6 (基数: 0.5)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t>t &gt; 6 (基数: 0)</t>
     </r>
   </si>
   <si>
@@ -176,7 +232,7 @@
   </si>
   <si>
     <t>分值=（转需求bug数+挂产品/项目身上bug数+转研发任务bug数）*3
-该项分值上限20分。</t>
+该项分值上限30分。</t>
   </si>
   <si>
     <t>用例发现Bug率</t>
@@ -1983,7 +2039,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="21">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E6" t="s" s="28">
         <v>21</v>
@@ -2064,7 +2120,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="21">
         <f>SUM(D4:D7)</f>
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>

</xml_diff>